<commit_message>
fixed request max pt to portion, errors for real network
</commit_message>
<xml_diff>
--- a/Data/Benchmark Lines/realeucmore.xlsx
+++ b/Data/Benchmark Lines/realeucmore.xlsx
@@ -1,20 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E62365-A5CE-478C-96B1-BBF4CBECBE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinates" sheetId="1" r:id="rId1"/>
     <sheet name="Stopinfo" sheetId="3" r:id="rId2"/>
     <sheet name="Distance" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -56,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,7 +138,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -153,7 +163,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-BE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -371,7 +381,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="459859440"/>
@@ -433,7 +443,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="459859112"/>
@@ -474,7 +484,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-BE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1058,7 +1068,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1338,20 +1354,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1363,7 +1379,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1385,7 +1401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1407,7 +1423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1430,7 +1446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1453,7 +1469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1476,7 +1492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1499,7 +1515,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1522,7 +1538,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1545,7 +1561,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1568,7 +1584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1591,7 +1607,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1614,7 +1630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1637,7 +1653,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1660,7 +1676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1683,7 +1699,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1706,14 +1722,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E17">
-        <f>SUM(E3:E16)</f>
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="N3:O16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N3:O16">
     <sortCondition descending="1" ref="N3:N16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1722,20 +1732,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1743,7 +1753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>16</v>
       </c>
@@ -1751,7 +1761,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>18</v>
       </c>
@@ -1759,7 +1769,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>21</v>
       </c>
@@ -1767,7 +1777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>22</v>
       </c>
@@ -1775,7 +1785,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>25</v>
       </c>
@@ -1783,7 +1793,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>26</v>
       </c>
@@ -1791,7 +1801,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>29</v>
       </c>
@@ -1799,12 +1809,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="B2:B10">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B10">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1812,21 +1822,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1843,7 +1853,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1860,7 +1870,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>3</v>
       </c>
@@ -1877,7 +1887,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -1894,7 +1904,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>6</v>
       </c>
@@ -1911,7 +1921,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>7</v>
       </c>
@@ -1928,7 +1938,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>8.5</v>
       </c>
@@ -1945,7 +1955,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>9.5</v>
       </c>
@@ -1962,7 +1972,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>11</v>
       </c>
@@ -1979,7 +1989,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>13</v>
       </c>
@@ -1996,7 +2006,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>15</v>
       </c>
@@ -2013,7 +2023,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>18</v>
       </c>
@@ -2030,7 +2040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>20.5</v>
       </c>
@@ -2047,7 +2057,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>24</v>
       </c>
@@ -2064,7 +2074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>27.5</v>
       </c>
@@ -2081,7 +2091,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>30</v>
       </c>
@@ -2098,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>32.5</v>
       </c>
@@ -2109,7 +2119,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>36</v>
       </c>
@@ -2118,7 +2128,7 @@
       </c>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>39.5</v>
       </c>
@@ -2129,7 +2139,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>42</v>
       </c>
@@ -2138,7 +2148,7 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45</v>
       </c>
@@ -2147,7 +2157,7 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>47</v>
       </c>
@@ -2158,7 +2168,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>49</v>
       </c>
@@ -2169,7 +2179,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>50.5</v>
       </c>
@@ -2178,7 +2188,7 @@
       </c>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>51.5</v>
       </c>
@@ -2187,7 +2197,7 @@
       </c>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>53</v>
       </c>
@@ -2198,7 +2208,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>54</v>
       </c>
@@ -2209,7 +2219,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>56</v>
       </c>
@@ -2218,7 +2228,7 @@
       </c>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>57</v>
       </c>
@@ -2227,7 +2237,7 @@
       </c>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>60</v>
       </c>
@@ -2238,11 +2248,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="B17:B32">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B17:B32">
     <sortCondition ref="B20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>